<commit_message>
FF: Restructured the code so that the slider no longer has to know about the Form class, and the survey.py module loops through the "response"s in the survey to capture all responses and score them appropriately.
Also now color questions that are compulsory in red if they are not answered when the user presses submit.
</commit_message>
<xml_diff>
--- a/psychopy/demos/coder/surveys/AQ.xlsx
+++ b/psychopy/demos/coder/surveys/AQ.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\antho\psychopy\psychopy\visual\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\antho\psychopy\psychopy\demos\coder\surveys\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{E5178734-444B-4CBB-A9D7-36D48FCD9112}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{4F853215-0A58-41AD-9C5F-4472506FDB91}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{BE50F44C-A788-4FF8-8131-E1E95C450F0F}"/>
   </bookViews>
@@ -123,15 +123,9 @@
     <t>AQ7</t>
   </si>
   <si>
-    <t>Other people frequently tell me that what I‚Äôve said is impolite, even though I think it is polite.</t>
-  </si>
-  <si>
     <t>AQ8</t>
   </si>
   <si>
-    <t>When I‚Äôm reading a story, I can easily imagine what the characters might look like.</t>
-  </si>
-  <si>
     <t>AQ9</t>
   </si>
   <si>
@@ -141,9 +135,6 @@
     <t>AQ10</t>
   </si>
   <si>
-    <t>In a social group, I can easily keep track of several different people‚Äôs conversations.</t>
-  </si>
-  <si>
     <t>AQ11</t>
   </si>
   <si>
@@ -177,9 +168,6 @@
     <t>AQ16</t>
   </si>
   <si>
-    <t>I tend to have very strong interests which I get upset about if I can‚Äôt pursue.</t>
-  </si>
-  <si>
     <t>AQ17</t>
   </si>
   <si>
@@ -189,9 +177,6 @@
     <t>AQ18</t>
   </si>
   <si>
-    <t>When I talk, it isn‚Äôt always easy for others to get a word in edgeways.</t>
-  </si>
-  <si>
     <t>AQ19</t>
   </si>
   <si>
@@ -201,15 +186,9 @@
     <t>AQ20</t>
   </si>
   <si>
-    <t>When I‚Äôm reading a story, I find it difficult to work out the characters‚Äô intentions.</t>
-  </si>
-  <si>
     <t>AQ21</t>
   </si>
   <si>
-    <t>I don‚Äôt particularly enjoy reading fiction.</t>
-  </si>
-  <si>
     <t>AQ22</t>
   </si>
   <si>
@@ -237,15 +216,9 @@
     <t>AQ26</t>
   </si>
   <si>
-    <t>I frequently find that I don‚Äôt know how to keep a conversation going.</t>
-  </si>
-  <si>
     <t>AQ27</t>
   </si>
   <si>
-    <t>I find it easy to ‚Äúread between the lines‚Äù when someone is talking to me.</t>
-  </si>
-  <si>
     <t>AQ28</t>
   </si>
   <si>
@@ -261,9 +234,6 @@
     <t>AQ30</t>
   </si>
   <si>
-    <t>I don‚Äôt usually notice small changes in a situation, or a person‚Äôs appearance.</t>
-  </si>
-  <si>
     <t>AQ31</t>
   </si>
   <si>
@@ -279,9 +249,6 @@
     <t>AQ33</t>
   </si>
   <si>
-    <t>When I talk on the phone, I‚Äôm not sure when it‚Äôs my turn to speak.</t>
-  </si>
-  <si>
     <t>AQ34</t>
   </si>
   <si>
@@ -351,9 +318,6 @@
     <t>AQ45</t>
   </si>
   <si>
-    <t>I find it difficult to work out people‚Äôs intentions.</t>
-  </si>
-  <si>
     <t>AQ46</t>
   </si>
   <si>
@@ -375,9 +339,6 @@
     <t>AQ49</t>
   </si>
   <si>
-    <t>I am not very good at remembering people‚Äôs date of birth.</t>
-  </si>
-  <si>
     <t>AQ50</t>
   </si>
   <si>
@@ -385,6 +346,45 @@
   </si>
   <si>
     <t>radio</t>
+  </si>
+  <si>
+    <t>Other people frequently tell me that what I've said is impolite, even though I think it is polite.</t>
+  </si>
+  <si>
+    <t>When I'm reading a story, I can easily imagine what the characters might look like.</t>
+  </si>
+  <si>
+    <t>In a social group, I can easily keep track of several different people's conversations.</t>
+  </si>
+  <si>
+    <t>I tend to have very strong interests which I get upset about if I can't pursue.</t>
+  </si>
+  <si>
+    <t>When I talk, it isn't always easy for others to get a word in edgeways.</t>
+  </si>
+  <si>
+    <t>When I'm reading a story, I find it difficult to work out the characters' intentions.</t>
+  </si>
+  <si>
+    <t>I don't particularly enjoy reading fiction.</t>
+  </si>
+  <si>
+    <t>I frequently find that I don't know how to keep a conversation going.</t>
+  </si>
+  <si>
+    <t>I don't usually notice small changes in a situation, or a person's appearance.</t>
+  </si>
+  <si>
+    <t>When I talk on the phone, I'm not sure when it's my turn to speak.</t>
+  </si>
+  <si>
+    <t>I find it difficult to work out people's intentions.</t>
+  </si>
+  <si>
+    <t>I am not very good at remembering people's date of birth.</t>
+  </si>
+  <si>
+    <t>I find it easy to "read between the lines" when someone is talking to me.</t>
   </si>
 </sst>
 </file>
@@ -738,11 +738,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4BEFC9E-C0FD-4BAD-B76B-20AF5BCAA15C}">
   <dimension ref="A1:L52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:L52"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="110.140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -801,7 +804,7 @@
         <v>16</v>
       </c>
       <c r="C3" t="s">
-        <v>119</v>
+        <v>106</v>
       </c>
       <c r="D3" t="s">
         <v>17</v>
@@ -827,7 +830,7 @@
         <v>22</v>
       </c>
       <c r="C4" t="s">
-        <v>119</v>
+        <v>106</v>
       </c>
       <c r="D4" t="s">
         <v>17</v>
@@ -853,7 +856,7 @@
         <v>24</v>
       </c>
       <c r="C5" t="s">
-        <v>119</v>
+        <v>106</v>
       </c>
       <c r="D5" t="s">
         <v>17</v>
@@ -879,7 +882,7 @@
         <v>26</v>
       </c>
       <c r="C6" t="s">
-        <v>119</v>
+        <v>106</v>
       </c>
       <c r="D6" t="s">
         <v>17</v>
@@ -905,7 +908,7 @@
         <v>28</v>
       </c>
       <c r="C7" t="s">
-        <v>119</v>
+        <v>106</v>
       </c>
       <c r="D7" t="s">
         <v>17</v>
@@ -931,7 +934,7 @@
         <v>30</v>
       </c>
       <c r="C8" t="s">
-        <v>119</v>
+        <v>106</v>
       </c>
       <c r="D8" t="s">
         <v>17</v>
@@ -954,10 +957,10 @@
         <v>31</v>
       </c>
       <c r="B9" t="s">
-        <v>32</v>
+        <v>107</v>
       </c>
       <c r="C9" t="s">
-        <v>119</v>
+        <v>106</v>
       </c>
       <c r="D9" t="s">
         <v>17</v>
@@ -977,13 +980,13 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B10" t="s">
-        <v>34</v>
+        <v>108</v>
       </c>
       <c r="C10" t="s">
-        <v>119</v>
+        <v>106</v>
       </c>
       <c r="D10" t="s">
         <v>17</v>
@@ -1003,13 +1006,13 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B11" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C11" t="s">
-        <v>119</v>
+        <v>106</v>
       </c>
       <c r="D11" t="s">
         <v>17</v>
@@ -1029,13 +1032,13 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B12" t="s">
-        <v>38</v>
+        <v>109</v>
       </c>
       <c r="C12" t="s">
-        <v>119</v>
+        <v>106</v>
       </c>
       <c r="D12" t="s">
         <v>17</v>
@@ -1055,13 +1058,13 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B13" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C13" t="s">
-        <v>119</v>
+        <v>106</v>
       </c>
       <c r="D13" t="s">
         <v>17</v>
@@ -1081,13 +1084,13 @@
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B14" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C14" t="s">
-        <v>119</v>
+        <v>106</v>
       </c>
       <c r="D14" t="s">
         <v>17</v>
@@ -1107,13 +1110,13 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B15" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C15" t="s">
-        <v>119</v>
+        <v>106</v>
       </c>
       <c r="D15" t="s">
         <v>17</v>
@@ -1133,13 +1136,13 @@
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B16" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C16" t="s">
-        <v>119</v>
+        <v>106</v>
       </c>
       <c r="D16" t="s">
         <v>17</v>
@@ -1159,13 +1162,13 @@
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B17" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C17" t="s">
-        <v>119</v>
+        <v>106</v>
       </c>
       <c r="D17" t="s">
         <v>17</v>
@@ -1185,13 +1188,13 @@
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B18" t="s">
-        <v>50</v>
+        <v>110</v>
       </c>
       <c r="C18" t="s">
-        <v>119</v>
+        <v>106</v>
       </c>
       <c r="D18" t="s">
         <v>17</v>
@@ -1211,13 +1214,13 @@
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B19" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C19" t="s">
-        <v>119</v>
+        <v>106</v>
       </c>
       <c r="D19" t="s">
         <v>17</v>
@@ -1237,13 +1240,13 @@
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B20" t="s">
-        <v>54</v>
+        <v>111</v>
       </c>
       <c r="C20" t="s">
-        <v>119</v>
+        <v>106</v>
       </c>
       <c r="D20" t="s">
         <v>17</v>
@@ -1263,13 +1266,13 @@
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="B21" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="C21" t="s">
-        <v>119</v>
+        <v>106</v>
       </c>
       <c r="D21" t="s">
         <v>17</v>
@@ -1289,13 +1292,13 @@
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="B22" t="s">
-        <v>58</v>
+        <v>112</v>
       </c>
       <c r="C22" t="s">
-        <v>119</v>
+        <v>106</v>
       </c>
       <c r="D22" t="s">
         <v>17</v>
@@ -1315,13 +1318,13 @@
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="B23" t="s">
-        <v>60</v>
+        <v>113</v>
       </c>
       <c r="C23" t="s">
-        <v>119</v>
+        <v>106</v>
       </c>
       <c r="D23" t="s">
         <v>17</v>
@@ -1341,13 +1344,13 @@
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="B24" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="C24" t="s">
-        <v>119</v>
+        <v>106</v>
       </c>
       <c r="D24" t="s">
         <v>17</v>
@@ -1367,13 +1370,13 @@
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="B25" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="C25" t="s">
-        <v>119</v>
+        <v>106</v>
       </c>
       <c r="D25" t="s">
         <v>17</v>
@@ -1393,13 +1396,13 @@
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="B26" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="C26" t="s">
-        <v>119</v>
+        <v>106</v>
       </c>
       <c r="D26" t="s">
         <v>17</v>
@@ -1419,13 +1422,13 @@
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="B27" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="C27" t="s">
-        <v>119</v>
+        <v>106</v>
       </c>
       <c r="D27" t="s">
         <v>17</v>
@@ -1445,13 +1448,13 @@
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="B28" t="s">
-        <v>70</v>
+        <v>114</v>
       </c>
       <c r="C28" t="s">
-        <v>119</v>
+        <v>106</v>
       </c>
       <c r="D28" t="s">
         <v>17</v>
@@ -1471,13 +1474,13 @@
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="B29" t="s">
-        <v>72</v>
+        <v>119</v>
       </c>
       <c r="C29" t="s">
-        <v>119</v>
+        <v>106</v>
       </c>
       <c r="D29" t="s">
         <v>17</v>
@@ -1497,13 +1500,13 @@
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="B30" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="C30" t="s">
-        <v>119</v>
+        <v>106</v>
       </c>
       <c r="D30" t="s">
         <v>17</v>
@@ -1523,13 +1526,13 @@
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="B31" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="C31" t="s">
-        <v>119</v>
+        <v>106</v>
       </c>
       <c r="D31" t="s">
         <v>17</v>
@@ -1549,13 +1552,13 @@
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="B32" t="s">
-        <v>78</v>
+        <v>115</v>
       </c>
       <c r="C32" t="s">
-        <v>119</v>
+        <v>106</v>
       </c>
       <c r="D32" t="s">
         <v>17</v>
@@ -1575,13 +1578,13 @@
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="B33" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="C33" t="s">
-        <v>119</v>
+        <v>106</v>
       </c>
       <c r="D33" t="s">
         <v>17</v>
@@ -1601,13 +1604,13 @@
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="B34" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="C34" t="s">
-        <v>119</v>
+        <v>106</v>
       </c>
       <c r="D34" t="s">
         <v>17</v>
@@ -1627,13 +1630,13 @@
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="B35" t="s">
-        <v>84</v>
+        <v>116</v>
       </c>
       <c r="C35" t="s">
-        <v>119</v>
+        <v>106</v>
       </c>
       <c r="D35" t="s">
         <v>17</v>
@@ -1653,13 +1656,13 @@
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="B36" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="C36" t="s">
-        <v>119</v>
+        <v>106</v>
       </c>
       <c r="D36" t="s">
         <v>17</v>
@@ -1679,13 +1682,13 @@
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="B37" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="C37" t="s">
-        <v>119</v>
+        <v>106</v>
       </c>
       <c r="D37" t="s">
         <v>17</v>
@@ -1705,13 +1708,13 @@
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="B38" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="C38" t="s">
-        <v>119</v>
+        <v>106</v>
       </c>
       <c r="D38" t="s">
         <v>17</v>
@@ -1731,13 +1734,13 @@
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="B39" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="C39" t="s">
-        <v>119</v>
+        <v>106</v>
       </c>
       <c r="D39" t="s">
         <v>17</v>
@@ -1757,13 +1760,13 @@
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="B40" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="C40" t="s">
-        <v>119</v>
+        <v>106</v>
       </c>
       <c r="D40" t="s">
         <v>17</v>
@@ -1783,13 +1786,13 @@
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
       <c r="B41" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="C41" t="s">
-        <v>119</v>
+        <v>106</v>
       </c>
       <c r="D41" t="s">
         <v>17</v>
@@ -1809,13 +1812,13 @@
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="B42" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
       <c r="C42" t="s">
-        <v>119</v>
+        <v>106</v>
       </c>
       <c r="D42" t="s">
         <v>17</v>
@@ -1835,13 +1838,13 @@
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="B43" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="C43" t="s">
-        <v>119</v>
+        <v>106</v>
       </c>
       <c r="D43" t="s">
         <v>17</v>
@@ -1861,13 +1864,13 @@
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
       <c r="B44" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="C44" t="s">
-        <v>119</v>
+        <v>106</v>
       </c>
       <c r="D44" t="s">
         <v>17</v>
@@ -1887,13 +1890,13 @@
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>103</v>
+        <v>92</v>
       </c>
       <c r="B45" t="s">
-        <v>104</v>
+        <v>93</v>
       </c>
       <c r="C45" t="s">
-        <v>119</v>
+        <v>106</v>
       </c>
       <c r="D45" t="s">
         <v>17</v>
@@ -1913,13 +1916,13 @@
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="B46" t="s">
-        <v>106</v>
+        <v>95</v>
       </c>
       <c r="C46" t="s">
-        <v>119</v>
+        <v>106</v>
       </c>
       <c r="D46" t="s">
         <v>17</v>
@@ -1939,13 +1942,13 @@
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>107</v>
+        <v>96</v>
       </c>
       <c r="B47" t="s">
-        <v>108</v>
+        <v>117</v>
       </c>
       <c r="C47" t="s">
-        <v>119</v>
+        <v>106</v>
       </c>
       <c r="D47" t="s">
         <v>17</v>
@@ -1965,13 +1968,13 @@
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>109</v>
+        <v>97</v>
       </c>
       <c r="B48" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="C48" t="s">
-        <v>119</v>
+        <v>106</v>
       </c>
       <c r="D48" t="s">
         <v>17</v>
@@ -1991,13 +1994,13 @@
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="B49" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="C49" t="s">
-        <v>119</v>
+        <v>106</v>
       </c>
       <c r="D49" t="s">
         <v>17</v>
@@ -2017,13 +2020,13 @@
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>113</v>
+        <v>101</v>
       </c>
       <c r="B50" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
       <c r="C50" t="s">
-        <v>119</v>
+        <v>106</v>
       </c>
       <c r="D50" t="s">
         <v>17</v>
@@ -2043,13 +2046,13 @@
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>115</v>
+        <v>103</v>
       </c>
       <c r="B51" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="C51" t="s">
-        <v>119</v>
+        <v>106</v>
       </c>
       <c r="D51" t="s">
         <v>17</v>
@@ -2069,13 +2072,13 @@
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>117</v>
+        <v>104</v>
       </c>
       <c r="B52" t="s">
-        <v>118</v>
+        <v>105</v>
       </c>
       <c r="C52" t="s">
-        <v>119</v>
+        <v>106</v>
       </c>
       <c r="D52" t="s">
         <v>17</v>

</xml_diff>